<commit_message>
Methoden für Flugzeuge und Flüge hinzugefügt. (siehe API_Methoden.xlsx)
Vererbung über DatabaseHandler.
</commit_message>
<xml_diff>
--- a/JavaEEProject/docs/API_Methoden.xlsx
+++ b/JavaEEProject/docs/API_Methoden.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <t>Klasse</t>
   </si>
@@ -142,12 +142,45 @@
   <si>
     <t>Methode, die zu einem Anmeldenamen den Nutzertypen ausgibt. Es sollte vorher die Methode checkPasswort ausgeführt werden.</t>
   </si>
+  <si>
+    <t>getAllRelationen</t>
+  </si>
+  <si>
+    <t>nicht implementiert</t>
+  </si>
+  <si>
+    <t>gibt alle Relationen aus. Beispiel:  "1. Relation: Startort: FRA, Zielort: BOM (1500 km, 10:30:00 Stunden)"</t>
+  </si>
+  <si>
+    <t>FlugzeugHandler</t>
+  </si>
+  <si>
+    <t>createFlugzeug</t>
+  </si>
+  <si>
+    <t>String hersteller, String typ, int sitzplaetze</t>
+  </si>
+  <si>
+    <t>"Erfolgreiche Anlage des Flugzeugs!"</t>
+  </si>
+  <si>
+    <t>"Bitte geben Sie alle Information an!"</t>
+  </si>
+  <si>
+    <t>getAllFlugzeuge</t>
+  </si>
+  <si>
+    <t>gibt alle Flugzeuge aus. Beispiel: "1. Flugzeug: Airbus A380-800 (853 Sitzplätze)"</t>
+  </si>
+  <si>
+    <t>assignFlugzeugToFlug</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +199,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -197,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -210,6 +250,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -494,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +548,7 @@
     <col min="3" max="3" width="34.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" customWidth="1"/>
     <col min="7" max="7" width="99.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -673,52 +716,94 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="G14" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>

</xml_diff>

<commit_message>
diverse Fehlerbehebungen/Erweiterungen (siehe API_Methoden.xlsx):
- Zuordnung Flug/Flugzeug möglich
- Anlage Flug möglich
- web.xml um Servlet erweitert
- Erstellung der Klasse SuccessHandler um Erfolgsmeldung zu
standardisieren und zu bündeln.
</commit_message>
<xml_diff>
--- a/JavaEEProject/docs/API_Methoden.xlsx
+++ b/JavaEEProject/docs/API_Methoden.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D390CD7C-72ED-4168-AE18-0A242EC593F0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>Klasse</t>
   </si>
@@ -116,6 +117,57 @@
   </si>
   <si>
     <t>Date abflug, Date ankunft, int relationid, double preis</t>
+  </si>
+  <si>
+    <t>getNutzertyp</t>
+  </si>
+  <si>
+    <t>String anmeldename</t>
+  </si>
+  <si>
+    <t>Methode, die zu einem Anmeldenamen den Nutzertypen ausgibt. Es sollte vorher die Methode checkPasswort ausgeführt werden.</t>
+  </si>
+  <si>
+    <t>getAllRelationen</t>
+  </si>
+  <si>
+    <t>nicht implementiert</t>
+  </si>
+  <si>
+    <t>gibt alle Relationen aus. Beispiel:  "1. Relation: Startort: FRA, Zielort: BOM (1500 km, 10:30:00 Stunden)"</t>
+  </si>
+  <si>
+    <t>FlugzeugHandler</t>
+  </si>
+  <si>
+    <t>createFlugzeug</t>
+  </si>
+  <si>
+    <t>String hersteller, String typ, int sitzplaetze</t>
+  </si>
+  <si>
+    <t>"Erfolgreiche Anlage des Flugzeugs!"</t>
+  </si>
+  <si>
+    <t>"Bitte geben Sie alle Information an!"</t>
+  </si>
+  <si>
+    <t>getAllFlugzeuge</t>
+  </si>
+  <si>
+    <t>assignFlugzeugToFlug</t>
+  </si>
+  <si>
+    <t>"Die Relation ist nicht vorhanden"</t>
+  </si>
+  <si>
+    <t>"Erfolgreiche Anlage des Flugs"</t>
+  </si>
+  <si>
+    <t>Methode, die eine Flug anlegt. Anfangs werden die Felder flugzeugid und mahlzeitid auf die default Felder der Tabellen Flugzeug und Mahlzeit belegt (jeweils die ID=1). Die FlugID setzt sich nach dem folgenden Muster zusammen: MH %relationid%/%flugnummer% (Die Flugnummer wird bei Neuanlage um 1 erhöht). Folglich hat der erste Flug der Relation 1  die FlugID MH1/1 der zweite Flug MH1/2 usw.</t>
+  </si>
+  <si>
+    <t>gellAllFluege</t>
   </si>
   <si>
     <r>
@@ -130,57 +182,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>String flugzeit im Format: "hh:mm:ss"</t>
+      <t>String flugzeit im Format: "hh:mm:ss". Startort und Zielort werden als Flughafennamen übergeben, aber mit der FlughafenID gespeichert!</t>
     </r>
   </si>
   <si>
-    <t>getNutzertyp</t>
-  </si>
-  <si>
-    <t>String anmeldename</t>
-  </si>
-  <si>
-    <t>Methode, die zu einem Anmeldenamen den Nutzertypen ausgibt. Es sollte vorher die Methode checkPasswort ausgeführt werden.</t>
-  </si>
-  <si>
-    <t>getAllRelationen</t>
-  </si>
-  <si>
-    <t>nicht implementiert</t>
-  </si>
-  <si>
-    <t>gibt alle Relationen aus. Beispiel:  "1. Relation: Startort: FRA, Zielort: BOM (1500 km, 10:30:00 Stunden)"</t>
-  </si>
-  <si>
-    <t>FlugzeugHandler</t>
-  </si>
-  <si>
-    <t>createFlugzeug</t>
-  </si>
-  <si>
-    <t>String hersteller, String typ, int sitzplaetze</t>
-  </si>
-  <si>
-    <t>"Erfolgreiche Anlage des Flugzeugs!"</t>
-  </si>
-  <si>
-    <t>"Bitte geben Sie alle Information an!"</t>
-  </si>
-  <si>
-    <t>getAllFlugzeuge</t>
-  </si>
-  <si>
-    <t>gibt alle Flugzeuge aus. Beispiel: "1. Flugzeug: Airbus A380-800 (853 Sitzplätze)"</t>
-  </si>
-  <si>
-    <t>assignFlugzeugToFlug</t>
+    <t>gibt alle Flugzeuge aus. Beispiel: "1. Flugzeug: Airbus A380-800 (853 Sitzplätze)" der Default Wert mit der flugzeugid=1 wird nicht ausgegeben. Der erste angezeigt Eintrag ist der zweite in der Datenbank. (Es wird auch mit 1. Flugzeug begonnen)</t>
+  </si>
+  <si>
+    <t>int flugzeugid, String flugid</t>
+  </si>
+  <si>
+    <t>Erfolgreiche Zuordnung!</t>
+  </si>
+  <si>
+    <t>Methode, die ein Flugzeug einem Flug zuordnet.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +228,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -237,7 +265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -251,9 +279,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
@@ -534,11 +566,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,10 +653,10 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
         <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -636,7 +668,7 @@
         <v>21</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -667,8 +699,8 @@
       <c r="F6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>31</v>
+      <c r="G6" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -701,7 +733,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -714,16 +746,20 @@
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="5" t="s">
-        <v>36</v>
+      <c r="E9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>21</v>
@@ -738,81 +774,88 @@
         <v>21</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="5" t="s">
-        <v>36</v>
+        <v>42</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>

</xml_diff>

<commit_message>
Mahlzeit implementiert (siehe API_Methoden.xlsx):
Anlage einer Mahlzeit
Ausgabe aller Mahlzeiten
Zuordnung einer Mahlzeit zu einem Flug
</commit_message>
<xml_diff>
--- a/JavaEEProject/docs/API_Methoden.xlsx
+++ b/JavaEEProject/docs/API_Methoden.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D390CD7C-72ED-4168-AE18-0A242EC593F0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{10C6D01F-05F1-4A26-A574-57B07643A42B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
   <si>
     <t>Klasse</t>
   </si>
@@ -81,9 +81,6 @@
     <t xml:space="preserve">  - "Relation schon vorhanden."
   - "Startort nicht gefunden."
   - "Zielort nicht gefunden."</t>
-  </si>
-  <si>
-    <t>Erfolgreiche Anlage der Relation.</t>
   </si>
   <si>
     <t>getAllFlughafennamen</t>
@@ -192,10 +189,52 @@
     <t>int flugzeugid, String flugid</t>
   </si>
   <si>
-    <t>Erfolgreiche Zuordnung!</t>
-  </si>
-  <si>
     <t>Methode, die ein Flugzeug einem Flug zuordnet.</t>
+  </si>
+  <si>
+    <t>MahlzeitHandler</t>
+  </si>
+  <si>
+    <t>createMahlzeit</t>
+  </si>
+  <si>
+    <t>String name, String art, Boolean vegetarisch</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - "Bitte geben Sie alle Information an!" - "Relation schon vorhanden."</t>
+  </si>
+  <si>
+    <t>"Erfolgreiche Anlage der Mahlzeit!"</t>
+  </si>
+  <si>
+    <t>getAllMahlzeiten</t>
+  </si>
+  <si>
+    <t>gibt alle Mahlzeiten aus. Beispiel: "1. Mahlzeit: Pizza Margarita (Teigwaren, vegetarisch: ja)" der Default Wert mit der mahlzeitid=1 wird nicht ausgegeben. Der erste angezeigt Eintrag ist der zweite in der Datenbank. (Es wird auch mit 1. Mahlzeit begonnen)</t>
+  </si>
+  <si>
+    <t>int mahlzeitid, String flugid</t>
+  </si>
+  <si>
+    <t>"Erfolgreiche Zuordnung des Flugzeugs!"</t>
+  </si>
+  <si>
+    <t>"Erfolgreiche Zuordnung der Mahlzeit!"</t>
+  </si>
+  <si>
+    <t>Methode, die eine Mahlzeit einem Flug zuordnet.</t>
+  </si>
+  <si>
+    <t>assignMahlzeitToFlug</t>
+  </si>
+  <si>
+    <t>Methode, die eine Mahlzeit anlegt.</t>
+  </si>
+  <si>
+    <t>Methode, die ein Flugzeug anlegt.</t>
+  </si>
+  <si>
+    <t>"Erfolgreiche Anlage der Relation!"</t>
   </si>
 </sst>
 </file>
@@ -569,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +619,7 @@
     <col min="3" max="3" width="34.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" customWidth="1"/>
+    <col min="6" max="6" width="37.5703125" customWidth="1"/>
     <col min="7" max="7" width="99.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -604,7 +643,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -627,7 +666,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -648,27 +687,27 @@
         <v>15</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -688,7 +727,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
@@ -697,31 +736,31 @@
         <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -735,54 +774,54 @@
     </row>
     <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -794,104 +833,142 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>41</v>
+      <c r="E13" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Passagier implementiert (siehe API_Methoden.xlsx):
Anlage eines Passagiers
Ausgabe aller Passagiere
</commit_message>
<xml_diff>
--- a/JavaEEProject/docs/API_Methoden.xlsx
+++ b/JavaEEProject/docs/API_Methoden.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{10C6D01F-05F1-4A26-A574-57B07643A42B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{AA9DC439-9CE7-4078-B567-F0A03327513A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
   <si>
     <t>Klasse</t>
   </si>
@@ -201,9 +201,6 @@
     <t>String name, String art, Boolean vegetarisch</t>
   </si>
   <si>
-    <t xml:space="preserve"> - "Bitte geben Sie alle Information an!" - "Relation schon vorhanden."</t>
-  </si>
-  <si>
     <t>"Erfolgreiche Anlage der Mahlzeit!"</t>
   </si>
   <si>
@@ -235,6 +232,30 @@
   </si>
   <si>
     <t>"Erfolgreiche Anlage der Relation!"</t>
+  </si>
+  <si>
+    <t>PassagierHandler</t>
+  </si>
+  <si>
+    <t>String vorname, String nachname, String anschrift, String geburtsdatum, String nationalitaet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - "Bitte geben Sie alle Information an!"                                                               - "Relation schon vorhanden."</t>
+  </si>
+  <si>
+    <t>"Erfolgreiche Anlage des Passagiers</t>
+  </si>
+  <si>
+    <t>Methode, die einen Passagier anlegt.</t>
+  </si>
+  <si>
+    <t>createPassagier</t>
+  </si>
+  <si>
+    <t>getAllPassagiere</t>
+  </si>
+  <si>
+    <t>gibt alle Passagier aus: Beispiel: "1. Passagier: Halil Özdogan (Anschrift: Am Stockhof 2, 31785 Hameln, Geburtsdatum: 08.09.1995, Nationalitaet: deutsch)"</t>
   </si>
 </sst>
 </file>
@@ -304,7 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -325,6 +346,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
@@ -606,19 +630,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" customWidth="1"/>
     <col min="6" max="6" width="37.5703125" customWidth="1"/>
     <col min="7" max="7" width="99.42578125" customWidth="1"/>
   </cols>
@@ -736,7 +760,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>47</v>
@@ -853,7 +877,7 @@
         <v>39</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -892,7 +916,7 @@
         <v>20</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>50</v>
@@ -921,21 +945,23 @@
         <v>9</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D18" s="1" t="s">
         <v>21</v>
       </c>
@@ -946,16 +972,16 @@
         <v>20</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>9</v>
@@ -964,10 +990,62 @@
         <v>20</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>61</v>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Buchungen implementiert (siehe API_Methoden.xlsx):
- Buchungen anlegen
- Buchungen zu Flügen ausgeben
- Buchungen zu Passagieren ausgeben

FlugHandler:
- Errechnen der Ankunftszeit aus der Abflugszeit (pom.xml:
commons-lang3)
- getAllFlugModels() -> für Anzeige aller Flüge und diverser
Informationen

alle DatabaseHandler:
- anstelle der direkten Übergabe einer ID (int oder String), wird mit
der Übergabe eines Strings in Form der getter-Methoden, der jeweiligen
Klasse gearbeitet.

Erweiterungen der Entities um Namedqueries und Update einzeler Entities.
Erweiterung SuccessHandler.
</commit_message>
<xml_diff>
--- a/JavaEEProject/docs/API_Methoden.xlsx
+++ b/JavaEEProject/docs/API_Methoden.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{AA9DC439-9CE7-4078-B567-F0A03327513A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{4A2D2C80-4A83-4F43-A143-C2E2DA94225D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
   <si>
     <t>Klasse</t>
   </si>
@@ -113,9 +113,6 @@
     <t>String startort, String zielort, String flugzeit, int distanz</t>
   </si>
   <si>
-    <t>Date abflug, Date ankunft, int relationid, double preis</t>
-  </si>
-  <si>
     <t>getNutzertyp</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>getAllRelationen</t>
   </si>
   <si>
-    <t>nicht implementiert</t>
-  </si>
-  <si>
     <t>gibt alle Relationen aus. Beispiel:  "1. Relation: Startort: FRA, Zielort: BOM (1500 km, 10:30:00 Stunden)"</t>
   </si>
   <si>
@@ -159,9 +153,6 @@
   </si>
   <si>
     <t>"Erfolgreiche Anlage des Flugs"</t>
-  </si>
-  <si>
-    <t>Methode, die eine Flug anlegt. Anfangs werden die Felder flugzeugid und mahlzeitid auf die default Felder der Tabellen Flugzeug und Mahlzeit belegt (jeweils die ID=1). Die FlugID setzt sich nach dem folgenden Muster zusammen: MH %relationid%/%flugnummer% (Die Flugnummer wird bei Neuanlage um 1 erhöht). Folglich hat der erste Flug der Relation 1  die FlugID MH1/1 der zweite Flug MH1/2 usw.</t>
   </si>
   <si>
     <t>gellAllFluege</t>
@@ -186,9 +177,6 @@
     <t>gibt alle Flugzeuge aus. Beispiel: "1. Flugzeug: Airbus A380-800 (853 Sitzplätze)" der Default Wert mit der flugzeugid=1 wird nicht ausgegeben. Der erste angezeigt Eintrag ist der zweite in der Datenbank. (Es wird auch mit 1. Flugzeug begonnen)</t>
   </si>
   <si>
-    <t>int flugzeugid, String flugid</t>
-  </si>
-  <si>
     <t>Methode, die ein Flugzeug einem Flug zuordnet.</t>
   </si>
   <si>
@@ -210,9 +198,6 @@
     <t>gibt alle Mahlzeiten aus. Beispiel: "1. Mahlzeit: Pizza Margarita (Teigwaren, vegetarisch: ja)" der Default Wert mit der mahlzeitid=1 wird nicht ausgegeben. Der erste angezeigt Eintrag ist der zweite in der Datenbank. (Es wird auch mit 1. Mahlzeit begonnen)</t>
   </si>
   <si>
-    <t>int mahlzeitid, String flugid</t>
-  </si>
-  <si>
     <t>"Erfolgreiche Zuordnung des Flugzeugs!"</t>
   </si>
   <si>
@@ -240,9 +225,6 @@
     <t>String vorname, String nachname, String anschrift, String geburtsdatum, String nationalitaet</t>
   </si>
   <si>
-    <t xml:space="preserve"> - "Bitte geben Sie alle Information an!"                                                               - "Relation schon vorhanden."</t>
-  </si>
-  <si>
     <t>"Erfolgreiche Anlage des Passagiers</t>
   </si>
   <si>
@@ -256,6 +238,87 @@
   </si>
   <si>
     <t>gibt alle Passagier aus: Beispiel: "1. Passagier: Halil Özdogan (Anschrift: Am Stockhof 2, 31785 Hameln, Geburtsdatum: 08.09.1995, Nationalitaet: deutsch)"</t>
+  </si>
+  <si>
+    <t>String abflug, String relationString, double preis</t>
+  </si>
+  <si>
+    <r>
+      <t>Methode, die eine Flug anlegt. Anfangs werden die Felder flugzeugid und mahlzeitid auf die default Felder der Tabellen Flugzeug und Mahlzeit belegt (jeweils die ID=1). Die FlugID setzt sich nach dem folgenden Muster zusammen: MH %relationid%/%flugnummer% (Die Flugnummer wird bei Neuanlage um 1 erhöht). Folglich hat der erste Flug der Relation 1  die FlugID MH1/1 der zweite Flug MH1/2 usw. Der String Abflug muss im Format</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> yyyy-mm-dd HH:mm </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sein.</t>
+    </r>
+  </si>
+  <si>
+    <t>gibt alle Flüge aus. Beispiel:  "MH1/1: Abflug: 2018-26-01 01:26, Ankunft: 2018-26-01 01:26 (Preis: 25.00 €)"</t>
+  </si>
+  <si>
+    <t>String flugzeugString, String flugString</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - "Bitte geben Sie alle Information an!"                                                               - "Mahlzeit schon vorhanden."</t>
+  </si>
+  <si>
+    <t>String mahlzeitString, String flugString</t>
+  </si>
+  <si>
+    <t>BuchungHandler</t>
+  </si>
+  <si>
+    <t>createBuchung</t>
+  </si>
+  <si>
+    <t>getBuchungenbyFlug</t>
+  </si>
+  <si>
+    <t>getBuchungenbyPassagier</t>
+  </si>
+  <si>
+    <t>Methode, die eine Buchung anlegt. Das Feld Buchungsdatum wird auf den Zeitpunkt der Buchung gesetzt.</t>
+  </si>
+  <si>
+    <t>"Erfolgreiche Anlage der Buchung!"</t>
+  </si>
+  <si>
+    <t>String passagierString, String flugString</t>
+  </si>
+  <si>
+    <t>String flugString</t>
+  </si>
+  <si>
+    <t>String passagierString</t>
+  </si>
+  <si>
+    <t>Methode, die alle Buchungen zu einem Flug ausgibt. Beispiel: 1. Buchung am Mon Apr 02 00:47:35 CEST 2018, Flug: MH1/4, Passagier: Halil Özdogan</t>
+  </si>
+  <si>
+    <t>Methode, die alle Buchungen zu einem Passagier ausgibt. Beispiel: 1. Buchung am Mon Apr 02 00:47:35 CEST 2018, Flug: MH1/4, Passagier: Halil Özdogan</t>
+  </si>
+  <si>
+    <t>getAllFlugModels</t>
+  </si>
+  <si>
+    <t>List&lt;FlugModel&gt;</t>
+  </si>
+  <si>
+    <t>Gibt eine Liste von Typ FlugModel zurück</t>
   </si>
 </sst>
 </file>
@@ -287,12 +350,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -325,7 +388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -336,18 +399,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -630,43 +692,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="31.42578125" customWidth="1"/>
     <col min="6" max="6" width="37.5703125" customWidth="1"/>
     <col min="7" max="7" width="99.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -715,23 +777,24 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -760,10 +823,10 @@
         <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -796,7 +859,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -804,25 +867,25 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>20</v>
@@ -837,215 +900,323 @@
         <v>20</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="E18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="E22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="C23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="1" t="s">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="E25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>72</v>
+      <c r="E26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Berechnen der Kapazitaet eines Flugs
</commit_message>
<xml_diff>
--- a/JavaEEProject/docs/API_Methoden.xlsx
+++ b/JavaEEProject/docs/API_Methoden.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{4A2D2C80-4A83-4F43-A143-C2E2DA94225D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{1106674C-D495-4C31-B542-098AE9FB53E4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="90">
   <si>
     <t>Klasse</t>
   </si>
@@ -319,6 +319,15 @@
   </si>
   <si>
     <t>Gibt eine Liste von Typ FlugModel zurück</t>
+  </si>
+  <si>
+    <t>calculateCapacity</t>
+  </si>
+  <si>
+    <t>Dieser Flug hat noch kein zugeordnetes Flugzeug!</t>
+  </si>
+  <si>
+    <t>gibt die Kapazität eines Flugs aus. Beispiel: Es sind noch 842 Plaetze von 853 Plaetzen frei.</t>
   </si>
 </sst>
 </file>
@@ -388,7 +397,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -410,6 +419,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -692,21 +704,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" customWidth="1"/>
-    <col min="6" max="6" width="37.5703125" customWidth="1"/>
-    <col min="7" max="7" width="99.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="112" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -755,7 +767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>12</v>
@@ -859,7 +871,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -953,7 +965,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
@@ -976,7 +988,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>39</v>
@@ -1154,7 +1166,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>73</v>
       </c>
@@ -1217,6 +1229,26 @@
       </c>
       <c r="G27" s="7" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Anpassung Ausgabe der Kapazitaet
</commit_message>
<xml_diff>
--- a/JavaEEProject/docs/API_Methoden.xlsx
+++ b/JavaEEProject/docs/API_Methoden.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{1106674C-D495-4C31-B542-098AE9FB53E4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C46B1DAD-C82A-40BB-9374-103E69A424FB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -327,7 +327,7 @@
     <t>Dieser Flug hat noch kein zugeordnetes Flugzeug!</t>
   </si>
   <si>
-    <t>gibt die Kapazität eines Flugs aus. Beispiel: Es sind noch 842 Plaetze von 853 Plaetzen frei.</t>
+    <t>gibt die Kapazität eines Flugs aus. Beispiel: 842 von 853 Plaetzen noch frei.</t>
   </si>
 </sst>
 </file>
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Setzen des Status zu einem Flug (FlugHandler getFlugStatus())
 & erste Dokumentation
</commit_message>
<xml_diff>
--- a/JavaEEProject/docs/API_Methoden.xlsx
+++ b/JavaEEProject/docs/API_Methoden.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C46B1DAD-C82A-40BB-9374-103E69A424FB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{7A22FCA0-9089-4907-AE2F-2E95149C1038}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="95">
   <si>
     <t>Klasse</t>
   </si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>gibt alle Flugzeuge aus. Beispiel: "1. Flugzeug: Airbus A380-800 (853 Sitzplätze)" der Default Wert mit der flugzeugid=1 wird nicht ausgegeben. Der erste angezeigt Eintrag ist der zweite in der Datenbank. (Es wird auch mit 1. Flugzeug begonnen)</t>
-  </si>
-  <si>
-    <t>Methode, die ein Flugzeug einem Flug zuordnet.</t>
   </si>
   <si>
     <t>MahlzeitHandler</t>
@@ -328,6 +325,24 @@
   </si>
   <si>
     <t>gibt die Kapazität eines Flugs aus. Beispiel: 842 von 853 Plaetzen noch frei.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - "Dieses Flugzeug wurde bereits einem Flug zugeordnet."                              - "Dieser Flugzeug wurde bereits diesem Flug zugeordnet."</t>
+  </si>
+  <si>
+    <t>Methode, die ein Flugzeug einem Flug zuordnet. Zu beachten ist, dass ein Flugzeug nur genau einem Flug zugeordnet werden kann!</t>
+  </si>
+  <si>
+    <t>getFlugstatus</t>
+  </si>
+  <si>
+    <t>String aktuellString, String flugstring</t>
+  </si>
+  <si>
+    <t>"Der Status kann nicht gesetzt werden."</t>
+  </si>
+  <si>
+    <t>Ausgabe des Status eines Flugs zu einer gegebeben Uhrzeit</t>
   </si>
 </sst>
 </file>
@@ -704,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,7 +731,7 @@
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" customWidth="1"/>
     <col min="6" max="6" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="112" bestFit="1" customWidth="1"/>
   </cols>
@@ -835,7 +850,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>44</v>
@@ -879,7 +894,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
@@ -891,7 +906,7 @@
         <v>42</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -933,290 +948,289 @@
         <v>20</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="B13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="B26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G25" s="1" t="s">
+      <c r="F26" s="6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>82</v>
+      <c r="G26" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>21</v>
@@ -1228,27 +1242,48 @@
         <v>20</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
       <c r="B28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C28" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="8" t="s">
+      <c r="F29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Überarbeitung der Methode createFlug
(Abflug wird im richtigen Format akzeptiert)
</commit_message>
<xml_diff>
--- a/JavaEEProject/docs/API_Methoden.xlsx
+++ b/JavaEEProject/docs/API_Methoden.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{7A22FCA0-9089-4907-AE2F-2E95149C1038}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{54108B0A-EA8A-41FE-902D-C136AF915406}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -240,6 +240,87 @@
     <t>String abflug, String relationString, double preis</t>
   </si>
   <si>
+    <t>gibt alle Flüge aus. Beispiel:  "MH1/1: Abflug: 2018-26-01 01:26, Ankunft: 2018-26-01 01:26 (Preis: 25.00 €)"</t>
+  </si>
+  <si>
+    <t>String flugzeugString, String flugString</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - "Bitte geben Sie alle Information an!"                                                               - "Mahlzeit schon vorhanden."</t>
+  </si>
+  <si>
+    <t>String mahlzeitString, String flugString</t>
+  </si>
+  <si>
+    <t>BuchungHandler</t>
+  </si>
+  <si>
+    <t>createBuchung</t>
+  </si>
+  <si>
+    <t>getBuchungenbyFlug</t>
+  </si>
+  <si>
+    <t>getBuchungenbyPassagier</t>
+  </si>
+  <si>
+    <t>Methode, die eine Buchung anlegt. Das Feld Buchungsdatum wird auf den Zeitpunkt der Buchung gesetzt.</t>
+  </si>
+  <si>
+    <t>"Erfolgreiche Anlage der Buchung!"</t>
+  </si>
+  <si>
+    <t>String passagierString, String flugString</t>
+  </si>
+  <si>
+    <t>String flugString</t>
+  </si>
+  <si>
+    <t>String passagierString</t>
+  </si>
+  <si>
+    <t>Methode, die alle Buchungen zu einem Flug ausgibt. Beispiel: 1. Buchung am Mon Apr 02 00:47:35 CEST 2018, Flug: MH1/4, Passagier: Halil Özdogan</t>
+  </si>
+  <si>
+    <t>Methode, die alle Buchungen zu einem Passagier ausgibt. Beispiel: 1. Buchung am Mon Apr 02 00:47:35 CEST 2018, Flug: MH1/4, Passagier: Halil Özdogan</t>
+  </si>
+  <si>
+    <t>getAllFlugModels</t>
+  </si>
+  <si>
+    <t>List&lt;FlugModel&gt;</t>
+  </si>
+  <si>
+    <t>Gibt eine Liste von Typ FlugModel zurück</t>
+  </si>
+  <si>
+    <t>calculateCapacity</t>
+  </si>
+  <si>
+    <t>Dieser Flug hat noch kein zugeordnetes Flugzeug!</t>
+  </si>
+  <si>
+    <t>gibt die Kapazität eines Flugs aus. Beispiel: 842 von 853 Plaetzen noch frei.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - "Dieses Flugzeug wurde bereits einem Flug zugeordnet."                              - "Dieser Flugzeug wurde bereits diesem Flug zugeordnet."</t>
+  </si>
+  <si>
+    <t>Methode, die ein Flugzeug einem Flug zuordnet. Zu beachten ist, dass ein Flugzeug nur genau einem Flug zugeordnet werden kann!</t>
+  </si>
+  <si>
+    <t>getFlugstatus</t>
+  </si>
+  <si>
+    <t>String aktuellString, String flugstring</t>
+  </si>
+  <si>
+    <t>"Der Status kann nicht gesetzt werden."</t>
+  </si>
+  <si>
+    <t>Ausgabe des Status eines Flugs zu einer gegebeben Uhrzeit</t>
+  </si>
+  <si>
     <r>
       <t>Methode, die eine Flug anlegt. Anfangs werden die Felder flugzeugid und mahlzeitid auf die default Felder der Tabellen Flugzeug und Mahlzeit belegt (jeweils die ID=1). Die FlugID setzt sich nach dem folgenden Muster zusammen: MH %relationid%/%flugnummer% (Die Flugnummer wird bei Neuanlage um 1 erhöht). Folglich hat der erste Flug der Relation 1  die FlugID MH1/1 der zweite Flug MH1/2 usw. Der String Abflug muss im Format</t>
     </r>
@@ -251,7 +332,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> yyyy-mm-dd HH:mm </t>
+      <t xml:space="preserve">"Tue Apr 17 17:46:00 CEST 2018" </t>
     </r>
     <r>
       <rPr>
@@ -262,87 +343,6 @@
       </rPr>
       <t>sein.</t>
     </r>
-  </si>
-  <si>
-    <t>gibt alle Flüge aus. Beispiel:  "MH1/1: Abflug: 2018-26-01 01:26, Ankunft: 2018-26-01 01:26 (Preis: 25.00 €)"</t>
-  </si>
-  <si>
-    <t>String flugzeugString, String flugString</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - "Bitte geben Sie alle Information an!"                                                               - "Mahlzeit schon vorhanden."</t>
-  </si>
-  <si>
-    <t>String mahlzeitString, String flugString</t>
-  </si>
-  <si>
-    <t>BuchungHandler</t>
-  </si>
-  <si>
-    <t>createBuchung</t>
-  </si>
-  <si>
-    <t>getBuchungenbyFlug</t>
-  </si>
-  <si>
-    <t>getBuchungenbyPassagier</t>
-  </si>
-  <si>
-    <t>Methode, die eine Buchung anlegt. Das Feld Buchungsdatum wird auf den Zeitpunkt der Buchung gesetzt.</t>
-  </si>
-  <si>
-    <t>"Erfolgreiche Anlage der Buchung!"</t>
-  </si>
-  <si>
-    <t>String passagierString, String flugString</t>
-  </si>
-  <si>
-    <t>String flugString</t>
-  </si>
-  <si>
-    <t>String passagierString</t>
-  </si>
-  <si>
-    <t>Methode, die alle Buchungen zu einem Flug ausgibt. Beispiel: 1. Buchung am Mon Apr 02 00:47:35 CEST 2018, Flug: MH1/4, Passagier: Halil Özdogan</t>
-  </si>
-  <si>
-    <t>Methode, die alle Buchungen zu einem Passagier ausgibt. Beispiel: 1. Buchung am Mon Apr 02 00:47:35 CEST 2018, Flug: MH1/4, Passagier: Halil Özdogan</t>
-  </si>
-  <si>
-    <t>getAllFlugModels</t>
-  </si>
-  <si>
-    <t>List&lt;FlugModel&gt;</t>
-  </si>
-  <si>
-    <t>Gibt eine Liste von Typ FlugModel zurück</t>
-  </si>
-  <si>
-    <t>calculateCapacity</t>
-  </si>
-  <si>
-    <t>Dieser Flug hat noch kein zugeordnetes Flugzeug!</t>
-  </si>
-  <si>
-    <t>gibt die Kapazität eines Flugs aus. Beispiel: 842 von 853 Plaetzen noch frei.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - "Dieses Flugzeug wurde bereits einem Flug zugeordnet."                              - "Dieser Flugzeug wurde bereits diesem Flug zugeordnet."</t>
-  </si>
-  <si>
-    <t>Methode, die ein Flugzeug einem Flug zuordnet. Zu beachten ist, dass ein Flugzeug nur genau einem Flug zugeordnet werden kann!</t>
-  </si>
-  <si>
-    <t>getFlugstatus</t>
-  </si>
-  <si>
-    <t>String aktuellString, String flugstring</t>
-  </si>
-  <si>
-    <t>"Der Status kann nicht gesetzt werden."</t>
-  </si>
-  <si>
-    <t>Ausgabe des Status eines Flugs zu einer gegebeben Uhrzeit</t>
   </si>
 </sst>
 </file>
@@ -721,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,7 +733,7 @@
     <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.7109375" customWidth="1"/>
     <col min="6" max="6" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="112" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="121.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -803,7 +803,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
         <v>29</v>
@@ -886,7 +886,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -906,7 +906,7 @@
         <v>42</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -948,47 +948,47 @@
         <v>20</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
         <v>91</v>
-      </c>
-      <c r="C13" t="s">
-        <v>92</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1050,19 +1050,19 @@
         <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1088,7 +1088,7 @@
         <v>9</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>49</v>
@@ -1124,7 +1124,7 @@
         <v>55</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>9</v>
@@ -1203,13 +1203,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="C26" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>9</v>
@@ -1218,19 +1218,19 @@
         <v>38</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>21</v>
@@ -1242,16 +1242,16 @@
         <v>20</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>21</v>
@@ -1263,27 +1263,27 @@
         <v>20</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E29" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>